<commit_message>
LCFS edits from WRI
</commit_message>
<xml_diff>
--- a/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
+++ b/InputData/trans/BVTStL/Boolean Veh Types Subject to LCFS.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\trans\BVTStL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C492B88C-673A-49AF-9C36-75D7567C6255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC0452BA-DF5F-456C-BE82-85A55BE60C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="260" windowWidth="19190" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BVTStL" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Source:</t>
   </si>
@@ -121,10 +121,7 @@
     <t xml:space="preserve">Sources are listed for reference. </t>
   </si>
   <si>
-    <t>We include railways as it is listed as one of the implementing ministries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in the National Biofuel Policy document. </t>
+    <t>We therefore exclude railways.</t>
   </si>
 </sst>
 </file>
@@ -535,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,11 +623,6 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -670,7 +662,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,10 +721,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>